<commit_message>
Added the remove empty delivery date function
</commit_message>
<xml_diff>
--- a/Vehicle information_20240728_213917.xlsx
+++ b/Vehicle information_20240728_213917.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97211\Desktop\Personal Stuff\SideProject\SideProj_excelSorting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7327ACC7-598B-41D0-9886-54F3F30C2218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7BB6C8-2529-4FD7-B46D-8489E475B99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle information" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6642" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6621" uniqueCount="779">
   <si>
     <t>Customer number</t>
   </si>
@@ -2788,7 +2788,7 @@
   <dimension ref="A1:AC291"/>
   <sheetViews>
     <sheetView topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -22823,10 +22823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D291"/>
+  <dimension ref="A1:D284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="A216" sqref="A216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22834,7 +22834,6 @@
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -22965,35 +22964,41 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
         <v>39</v>
@@ -23001,13 +23006,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
         <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -23015,13 +23020,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
@@ -23029,13 +23034,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
         <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D15" t="s">
         <v>39</v>
@@ -23043,13 +23048,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>
@@ -23057,13 +23062,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -23071,13 +23076,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
         <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
         <v>39</v>
@@ -23085,13 +23090,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
         <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -23099,13 +23104,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
         <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D20" t="s">
         <v>39</v>
@@ -23113,27 +23118,27 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D22" t="s">
         <v>39</v>
@@ -23141,83 +23146,83 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D27" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D28" t="s">
         <v>39</v>
@@ -23225,13 +23230,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D29" t="s">
         <v>39</v>
@@ -23239,13 +23244,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>155</v>
       </c>
       <c r="D30" t="s">
         <v>39</v>
@@ -23253,13 +23258,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
         <v>39</v>
@@ -23267,27 +23272,27 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>155</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B33" t="s">
         <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="D33" t="s">
         <v>39</v>
@@ -23295,21 +23300,21 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B35" t="s">
         <v>69</v>
@@ -23323,13 +23328,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B36" t="s">
         <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>170</v>
       </c>
       <c r="D36" t="s">
         <v>39</v>
@@ -23337,13 +23342,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>162</v>
+        <v>61</v>
       </c>
       <c r="D37" t="s">
         <v>39</v>
@@ -23351,13 +23356,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B38" t="s">
         <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D38" t="s">
         <v>39</v>
@@ -23365,13 +23370,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B39" t="s">
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>177</v>
       </c>
       <c r="D39" t="s">
         <v>39</v>
@@ -23379,13 +23384,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B40" t="s">
         <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D40" t="s">
         <v>39</v>
@@ -23393,13 +23398,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B41" t="s">
         <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D41" t="s">
         <v>39</v>
@@ -23407,13 +23412,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B42" t="s">
         <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D42" t="s">
         <v>39</v>
@@ -23421,24 +23426,27 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>59</v>
+      </c>
+      <c r="C43" t="s">
+        <v>190</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>184</v>
+        <v>61</v>
       </c>
       <c r="D44" t="s">
         <v>39</v>
@@ -23446,27 +23454,27 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>186</v>
+        <v>40</v>
       </c>
       <c r="D45" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="B46" t="s">
         <v>59</v>
       </c>
       <c r="C46" t="s">
-        <v>190</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
         <v>39</v>
@@ -23474,13 +23482,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>200</v>
       </c>
       <c r="D47" t="s">
         <v>39</v>
@@ -23488,41 +23496,41 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>204</v>
       </c>
       <c r="D48" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>209</v>
       </c>
       <c r="C49" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="D49" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="D50" t="s">
         <v>39</v>
@@ -23530,41 +23538,41 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>204</v>
+        <v>37</v>
       </c>
       <c r="D51" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="B52" t="s">
-        <v>209</v>
+        <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>222</v>
       </c>
       <c r="D52" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C53" t="s">
-        <v>216</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
         <v>39</v>
@@ -23572,13 +23580,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="B54" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C54" t="s">
-        <v>37</v>
+        <v>233</v>
       </c>
       <c r="D54" t="s">
         <v>122</v>
@@ -23586,13 +23594,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B55" t="s">
         <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="D55" t="s">
         <v>39</v>
@@ -23600,24 +23608,27 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>69</v>
+      </c>
+      <c r="C56" t="s">
+        <v>99</v>
       </c>
       <c r="D56" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="B57" t="s">
         <v>69</v>
       </c>
       <c r="C57" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="D57" t="s">
         <v>39</v>
@@ -23625,27 +23636,27 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>233</v>
+        <v>177</v>
       </c>
       <c r="D58" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="B59" t="s">
         <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>186</v>
+        <v>105</v>
       </c>
       <c r="D59" t="s">
         <v>39</v>
@@ -23653,13 +23664,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>99</v>
+        <v>190</v>
       </c>
       <c r="D60" t="s">
         <v>39</v>
@@ -23667,13 +23678,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B61" t="s">
         <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>155</v>
+        <v>250</v>
       </c>
       <c r="D61" t="s">
         <v>39</v>
@@ -23681,27 +23692,27 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C62" t="s">
-        <v>177</v>
+        <v>52</v>
       </c>
       <c r="D62" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C63" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="D63" t="s">
         <v>39</v>
@@ -23709,13 +23720,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="B64" t="s">
         <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="D64" t="s">
         <v>39</v>
@@ -23723,13 +23734,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C65" t="s">
-        <v>250</v>
+        <v>151</v>
       </c>
       <c r="D65" t="s">
         <v>39</v>
@@ -23737,27 +23748,27 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="B66" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C66" t="s">
-        <v>52</v>
+        <v>265</v>
       </c>
       <c r="D66" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="B67" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
+        <v>268</v>
       </c>
       <c r="D67" t="s">
         <v>39</v>
@@ -23765,13 +23776,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="B68" t="s">
         <v>59</v>
       </c>
       <c r="C68" t="s">
-        <v>177</v>
+        <v>272</v>
       </c>
       <c r="D68" t="s">
         <v>39</v>
@@ -23779,13 +23790,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="B69" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="D69" t="s">
         <v>39</v>
@@ -23793,27 +23804,27 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="C70" t="s">
-        <v>265</v>
+        <v>52</v>
       </c>
       <c r="D70" t="s">
-        <v>122</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="B71" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="D71" t="s">
         <v>39</v>
@@ -23821,13 +23832,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>272</v>
+        <v>216</v>
       </c>
       <c r="D72" t="s">
         <v>39</v>
@@ -23835,13 +23846,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="B73" t="s">
-        <v>59</v>
+        <v>285</v>
       </c>
       <c r="C73" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="D73" t="s">
         <v>39</v>
@@ -23849,27 +23860,27 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="B74" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="C74" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="D74" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="D75" t="s">
         <v>39</v>
@@ -23877,13 +23888,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C76" t="s">
-        <v>216</v>
+        <v>295</v>
       </c>
       <c r="D76" t="s">
         <v>39</v>
@@ -23891,27 +23902,27 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="B77" t="s">
-        <v>285</v>
+        <v>48</v>
       </c>
       <c r="C77" t="s">
-        <v>128</v>
+        <v>37</v>
       </c>
       <c r="D77" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="B78" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="C78" t="s">
-        <v>93</v>
+        <v>302</v>
       </c>
       <c r="D78" t="s">
         <v>39</v>
@@ -23919,13 +23930,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>288</v>
+        <v>303</v>
       </c>
       <c r="B79" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C79" t="s">
-        <v>291</v>
+        <v>37</v>
       </c>
       <c r="D79" t="s">
         <v>39</v>
@@ -23933,13 +23944,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="B80" t="s">
         <v>59</v>
       </c>
       <c r="C80" t="s">
-        <v>295</v>
+        <v>75</v>
       </c>
       <c r="D80" t="s">
         <v>39</v>
@@ -23947,27 +23958,27 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="B81" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C81" t="s">
-        <v>37</v>
+        <v>308</v>
       </c>
       <c r="D81" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="B82" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C82" t="s">
-        <v>302</v>
+        <v>148</v>
       </c>
       <c r="D82" t="s">
         <v>39</v>
@@ -23975,13 +23986,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="B83" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C83" t="s">
-        <v>37</v>
+        <v>313</v>
       </c>
       <c r="D83" t="s">
         <v>39</v>
@@ -23989,13 +24000,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="B84" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C84" t="s">
-        <v>75</v>
+        <v>315</v>
       </c>
       <c r="D84" t="s">
         <v>39</v>
@@ -24003,13 +24014,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C85" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="D85" t="s">
         <v>39</v>
@@ -24017,13 +24028,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="B86" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C86" t="s">
-        <v>148</v>
+        <v>319</v>
       </c>
       <c r="D86" t="s">
         <v>39</v>
@@ -24031,55 +24042,55 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="B87" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C87" t="s">
-        <v>313</v>
+        <v>52</v>
       </c>
       <c r="D87" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="B88" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C88" t="s">
-        <v>315</v>
+        <v>37</v>
       </c>
       <c r="D88" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="B89" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C89" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="D89" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="B90" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C90" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="D90" t="s">
         <v>39</v>
@@ -24087,55 +24098,55 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="B91" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C91" t="s">
-        <v>52</v>
+        <v>335</v>
       </c>
       <c r="D91" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="B92" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C92" t="s">
-        <v>37</v>
+        <v>179</v>
       </c>
       <c r="D92" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="B93" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C93" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="D93" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="B94" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="C94" t="s">
-        <v>308</v>
+        <v>71</v>
       </c>
       <c r="D94" t="s">
         <v>39</v>
@@ -24143,27 +24154,27 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="B95" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C95" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="D95" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="B96" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C96" t="s">
-        <v>179</v>
+        <v>348</v>
       </c>
       <c r="D96" t="s">
         <v>39</v>
@@ -24171,13 +24182,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="B97" t="s">
         <v>59</v>
       </c>
       <c r="C97" t="s">
-        <v>341</v>
+        <v>175</v>
       </c>
       <c r="D97" t="s">
         <v>39</v>
@@ -24185,13 +24196,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="B98" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C98" t="s">
-        <v>71</v>
+        <v>353</v>
       </c>
       <c r="D98" t="s">
         <v>39</v>
@@ -24199,13 +24210,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>343</v>
+        <v>355</v>
       </c>
       <c r="B99" t="s">
         <v>59</v>
       </c>
       <c r="C99" t="s">
-        <v>344</v>
+        <v>113</v>
       </c>
       <c r="D99" t="s">
         <v>39</v>
@@ -24213,13 +24224,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
       <c r="B100" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C100" t="s">
-        <v>348</v>
+        <v>162</v>
       </c>
       <c r="D100" t="s">
         <v>39</v>
@@ -24227,13 +24238,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="B101" t="s">
         <v>59</v>
       </c>
       <c r="C101" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="D101" t="s">
         <v>39</v>
@@ -24241,13 +24252,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="B102" t="s">
         <v>59</v>
       </c>
       <c r="C102" t="s">
-        <v>353</v>
+        <v>151</v>
       </c>
       <c r="D102" t="s">
         <v>39</v>
@@ -24255,24 +24266,27 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="B103" t="s">
-        <v>78</v>
+        <v>366</v>
+      </c>
+      <c r="C103" t="s">
+        <v>45</v>
       </c>
       <c r="D103" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>355</v>
+        <v>371</v>
       </c>
       <c r="B104" t="s">
         <v>59</v>
       </c>
       <c r="C104" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D104" t="s">
         <v>39</v>
@@ -24280,13 +24294,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>356</v>
+        <v>372</v>
       </c>
       <c r="B105" t="s">
         <v>69</v>
       </c>
       <c r="C105" t="s">
-        <v>162</v>
+        <v>375</v>
       </c>
       <c r="D105" t="s">
         <v>39</v>
@@ -24294,13 +24308,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>357</v>
+        <v>376</v>
       </c>
       <c r="B106" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C106" t="s">
-        <v>155</v>
+        <v>308</v>
       </c>
       <c r="D106" t="s">
         <v>39</v>
@@ -24308,13 +24322,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>360</v>
+        <v>377</v>
       </c>
       <c r="B107" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C107" t="s">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="D107" t="s">
         <v>39</v>
@@ -24322,41 +24336,41 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>363</v>
+        <v>380</v>
       </c>
       <c r="B108" t="s">
-        <v>366</v>
+        <v>59</v>
       </c>
       <c r="C108" t="s">
-        <v>45</v>
+        <v>295</v>
       </c>
       <c r="D108" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="B109" t="s">
-        <v>59</v>
+        <v>366</v>
       </c>
       <c r="C109" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="D109" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="B110" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C110" t="s">
-        <v>375</v>
+        <v>348</v>
       </c>
       <c r="D110" t="s">
         <v>39</v>
@@ -24364,13 +24378,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="B111" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C111" t="s">
-        <v>308</v>
+        <v>162</v>
       </c>
       <c r="D111" t="s">
         <v>39</v>
@@ -24378,13 +24392,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="B112" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C112" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="D112" t="s">
         <v>39</v>
@@ -24392,13 +24406,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="B113" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C113" t="s">
-        <v>295</v>
+        <v>99</v>
       </c>
       <c r="D113" t="s">
         <v>39</v>
@@ -24406,27 +24420,27 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="B114" t="s">
-        <v>366</v>
+        <v>84</v>
       </c>
       <c r="C114" t="s">
-        <v>65</v>
+        <v>148</v>
       </c>
       <c r="D114" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="B115" t="s">
         <v>59</v>
       </c>
       <c r="C115" t="s">
-        <v>348</v>
+        <v>75</v>
       </c>
       <c r="D115" t="s">
         <v>39</v>
@@ -24434,13 +24448,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>385</v>
+        <v>400</v>
       </c>
       <c r="B116" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C116" t="s">
-        <v>162</v>
+        <v>37</v>
       </c>
       <c r="D116" t="s">
         <v>39</v>
@@ -24448,13 +24462,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>388</v>
+        <v>403</v>
       </c>
       <c r="B117" t="s">
         <v>35</v>
       </c>
       <c r="C117" t="s">
-        <v>128</v>
+        <v>375</v>
       </c>
       <c r="D117" t="s">
         <v>39</v>
@@ -24462,27 +24476,27 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>391</v>
+        <v>406</v>
       </c>
       <c r="B118" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C118" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="D118" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
       <c r="B119" t="s">
         <v>84</v>
       </c>
       <c r="C119" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="D119" t="s">
         <v>39</v>
@@ -24490,13 +24504,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="B120" t="s">
         <v>59</v>
       </c>
       <c r="C120" t="s">
-        <v>75</v>
+        <v>411</v>
       </c>
       <c r="D120" t="s">
         <v>39</v>
@@ -24504,13 +24518,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="B121" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C121" t="s">
-        <v>37</v>
+        <v>413</v>
       </c>
       <c r="D121" t="s">
         <v>39</v>
@@ -24518,13 +24532,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="B122" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C122" t="s">
-        <v>375</v>
+        <v>415</v>
       </c>
       <c r="D122" t="s">
         <v>39</v>
@@ -24532,27 +24546,27 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="B123" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C123" t="s">
-        <v>52</v>
+        <v>417</v>
       </c>
       <c r="D123" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="B124" t="s">
-        <v>84</v>
+        <v>285</v>
       </c>
       <c r="C124" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="D124" t="s">
         <v>39</v>
@@ -24560,13 +24574,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="B125" t="s">
         <v>59</v>
       </c>
       <c r="C125" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="D125" t="s">
         <v>39</v>
@@ -24574,13 +24588,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="B126" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C126" t="s">
-        <v>413</v>
+        <v>128</v>
       </c>
       <c r="D126" t="s">
         <v>39</v>
@@ -24588,21 +24602,21 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="B127" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C127" t="s">
-        <v>415</v>
+        <v>214</v>
       </c>
       <c r="D127" t="s">
-        <v>39</v>
+        <v>428</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>416</v>
+        <v>431</v>
       </c>
       <c r="B128" t="s">
         <v>59</v>
@@ -24616,10 +24630,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="B129" t="s">
-        <v>285</v>
+        <v>35</v>
       </c>
       <c r="C129" t="s">
         <v>128</v>
@@ -24630,13 +24644,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>420</v>
+        <v>435</v>
       </c>
       <c r="B130" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C130" t="s">
-        <v>421</v>
+        <v>186</v>
       </c>
       <c r="D130" t="s">
         <v>39</v>
@@ -24644,13 +24658,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>422</v>
+        <v>436</v>
       </c>
       <c r="B131" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="C131" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D131" t="s">
         <v>39</v>
@@ -24658,41 +24672,41 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>425</v>
+        <v>439</v>
       </c>
       <c r="B132" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C132" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="D132" t="s">
-        <v>428</v>
+        <v>39</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="B133" t="s">
-        <v>59</v>
+        <v>366</v>
       </c>
       <c r="C133" t="s">
-        <v>417</v>
+        <v>184</v>
       </c>
       <c r="D133" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="B134" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="C134" t="s">
-        <v>128</v>
+        <v>417</v>
       </c>
       <c r="D134" t="s">
         <v>39</v>
@@ -24700,13 +24714,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="B135" t="s">
         <v>84</v>
       </c>
       <c r="C135" t="s">
-        <v>186</v>
+        <v>44</v>
       </c>
       <c r="D135" t="s">
         <v>39</v>
@@ -24714,13 +24728,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="B136" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="C136" t="s">
-        <v>132</v>
+        <v>295</v>
       </c>
       <c r="D136" t="s">
         <v>39</v>
@@ -24728,41 +24742,41 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="B137" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C137" t="s">
-        <v>186</v>
+        <v>448</v>
       </c>
       <c r="D137" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="B138" t="s">
-        <v>366</v>
+        <v>59</v>
       </c>
       <c r="C138" t="s">
-        <v>184</v>
+        <v>453</v>
       </c>
       <c r="D138" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="B139" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C139" t="s">
-        <v>417</v>
+        <v>162</v>
       </c>
       <c r="D139" t="s">
         <v>39</v>
@@ -24770,27 +24784,27 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="B140" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C140" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D140" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="B141" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C141" t="s">
-        <v>295</v>
+        <v>109</v>
       </c>
       <c r="D141" t="s">
         <v>39</v>
@@ -24798,27 +24812,27 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="B142" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C142" t="s">
-        <v>448</v>
+        <v>278</v>
       </c>
       <c r="D142" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="B143" t="s">
         <v>59</v>
       </c>
       <c r="C143" t="s">
-        <v>453</v>
+        <v>421</v>
       </c>
       <c r="D143" t="s">
         <v>39</v>
@@ -24826,13 +24840,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="B144" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C144" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="D144" t="s">
         <v>39</v>
@@ -24840,27 +24854,27 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="B145" t="s">
-        <v>48</v>
+        <v>285</v>
       </c>
       <c r="C145" t="s">
-        <v>52</v>
+        <v>341</v>
       </c>
       <c r="D145" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="B146" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C146" t="s">
-        <v>109</v>
+        <v>162</v>
       </c>
       <c r="D146" t="s">
         <v>39</v>
@@ -24868,27 +24882,27 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="B147" t="s">
-        <v>59</v>
+        <v>366</v>
       </c>
       <c r="C147" t="s">
-        <v>278</v>
+        <v>470</v>
       </c>
       <c r="D147" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="B148" t="s">
         <v>59</v>
       </c>
       <c r="C148" t="s">
-        <v>421</v>
+        <v>107</v>
       </c>
       <c r="D148" t="s">
         <v>39</v>
@@ -24896,27 +24910,27 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="B149" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C149" t="s">
-        <v>177</v>
+        <v>52</v>
       </c>
       <c r="D149" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>462</v>
+        <v>477</v>
       </c>
       <c r="B150" t="s">
-        <v>285</v>
+        <v>59</v>
       </c>
       <c r="C150" t="s">
-        <v>341</v>
+        <v>99</v>
       </c>
       <c r="D150" t="s">
         <v>39</v>
@@ -24924,13 +24938,13 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>464</v>
+        <v>480</v>
       </c>
       <c r="B151" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C151" t="s">
-        <v>162</v>
+        <v>67</v>
       </c>
       <c r="D151" t="s">
         <v>39</v>
@@ -24938,27 +24952,27 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>467</v>
+        <v>483</v>
       </c>
       <c r="B152" t="s">
-        <v>366</v>
+        <v>35</v>
       </c>
       <c r="C152" t="s">
-        <v>470</v>
+        <v>484</v>
       </c>
       <c r="D152" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>474</v>
+        <v>485</v>
       </c>
       <c r="B153" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C153" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D153" t="s">
         <v>39</v>
@@ -24966,7 +24980,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="B154" t="s">
         <v>48</v>
@@ -24980,13 +24994,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="B155" t="s">
         <v>59</v>
       </c>
       <c r="C155" t="s">
-        <v>99</v>
+        <v>308</v>
       </c>
       <c r="D155" t="s">
         <v>39</v>
@@ -24994,13 +25008,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="B156" t="s">
         <v>59</v>
       </c>
       <c r="C156" t="s">
-        <v>67</v>
+        <v>353</v>
       </c>
       <c r="D156" t="s">
         <v>39</v>
@@ -25008,13 +25022,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
       <c r="B157" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C157" t="s">
-        <v>484</v>
+        <v>115</v>
       </c>
       <c r="D157" t="s">
         <v>39</v>
@@ -25022,13 +25036,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>485</v>
+        <v>494</v>
       </c>
       <c r="B158" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="C158" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="D158" t="s">
         <v>39</v>
@@ -25036,27 +25050,27 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>486</v>
+        <v>497</v>
       </c>
       <c r="B159" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C159" t="s">
-        <v>52</v>
+        <v>302</v>
       </c>
       <c r="D159" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>487</v>
+        <v>500</v>
       </c>
       <c r="B160" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C160" t="s">
-        <v>308</v>
+        <v>501</v>
       </c>
       <c r="D160" t="s">
         <v>39</v>
@@ -25064,13 +25078,13 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>488</v>
+        <v>502</v>
       </c>
       <c r="B161" t="s">
         <v>59</v>
       </c>
       <c r="C161" t="s">
-        <v>353</v>
+        <v>505</v>
       </c>
       <c r="D161" t="s">
         <v>39</v>
@@ -25078,27 +25092,27 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>491</v>
+        <v>509</v>
       </c>
       <c r="B162" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C162" t="s">
-        <v>115</v>
+        <v>511</v>
       </c>
       <c r="D162" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>494</v>
+        <v>515</v>
       </c>
       <c r="B163" t="s">
         <v>59</v>
       </c>
       <c r="C163" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="D163" t="s">
         <v>39</v>
@@ -25106,13 +25120,13 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>497</v>
+        <v>516</v>
       </c>
       <c r="B164" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C164" t="s">
-        <v>302</v>
+        <v>99</v>
       </c>
       <c r="D164" t="s">
         <v>39</v>
@@ -25120,13 +25134,13 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>500</v>
+        <v>517</v>
       </c>
       <c r="B165" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C165" t="s">
-        <v>501</v>
+        <v>105</v>
       </c>
       <c r="D165" t="s">
         <v>39</v>
@@ -25134,13 +25148,13 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>502</v>
+        <v>520</v>
       </c>
       <c r="B166" t="s">
         <v>59</v>
       </c>
       <c r="C166" t="s">
-        <v>505</v>
+        <v>71</v>
       </c>
       <c r="D166" t="s">
         <v>39</v>
@@ -25148,41 +25162,41 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>509</v>
+        <v>523</v>
       </c>
       <c r="B167" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C167" t="s">
-        <v>511</v>
+        <v>151</v>
       </c>
       <c r="D167" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>515</v>
+        <v>524</v>
       </c>
       <c r="B168" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C168" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D168" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="B169" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C169" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D169" t="s">
         <v>39</v>
@@ -25190,13 +25204,13 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>517</v>
+        <v>528</v>
       </c>
       <c r="B170" t="s">
         <v>59</v>
       </c>
       <c r="C170" t="s">
-        <v>105</v>
+        <v>222</v>
       </c>
       <c r="D170" t="s">
         <v>39</v>
@@ -25204,13 +25218,13 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="B171" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C171" t="s">
-        <v>71</v>
+        <v>162</v>
       </c>
       <c r="D171" t="s">
         <v>39</v>
@@ -25218,13 +25232,13 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="B172" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C172" t="s">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="D172" t="s">
         <v>39</v>
@@ -25232,27 +25246,27 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="B173" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C173" t="s">
-        <v>52</v>
+        <v>162</v>
       </c>
       <c r="D173" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>525</v>
+        <v>536</v>
       </c>
       <c r="B174" t="s">
         <v>59</v>
       </c>
       <c r="C174" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="D174" t="s">
         <v>39</v>
@@ -25260,13 +25274,13 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="B175" t="s">
         <v>59</v>
       </c>
       <c r="C175" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="D175" t="s">
         <v>39</v>
@@ -25274,13 +25288,13 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>529</v>
+        <v>540</v>
       </c>
       <c r="B176" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C176" t="s">
-        <v>162</v>
+        <v>417</v>
       </c>
       <c r="D176" t="s">
         <v>39</v>
@@ -25288,27 +25302,27 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>530</v>
+        <v>541</v>
       </c>
       <c r="B177" t="s">
-        <v>59</v>
+        <v>366</v>
       </c>
       <c r="C177" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="D177" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>533</v>
+        <v>543</v>
       </c>
       <c r="B178" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C178" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="D178" t="s">
         <v>39</v>
@@ -25316,13 +25330,13 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>536</v>
+        <v>544</v>
       </c>
       <c r="B179" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C179" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D179" t="s">
         <v>39</v>
@@ -25330,13 +25344,13 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="B180" t="s">
         <v>59</v>
       </c>
       <c r="C180" t="s">
-        <v>250</v>
+        <v>151</v>
       </c>
       <c r="D180" t="s">
         <v>39</v>
@@ -25344,13 +25358,13 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="B181" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C181" t="s">
-        <v>417</v>
+        <v>99</v>
       </c>
       <c r="D181" t="s">
         <v>39</v>
@@ -25358,27 +25372,27 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>541</v>
+        <v>551</v>
       </c>
       <c r="B182" t="s">
-        <v>366</v>
+        <v>69</v>
       </c>
       <c r="C182" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="D182" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>543</v>
+        <v>552</v>
       </c>
       <c r="B183" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C183" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="D183" t="s">
         <v>39</v>
@@ -25386,21 +25400,21 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>544</v>
+        <v>553</v>
       </c>
       <c r="B184" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C184" t="s">
-        <v>67</v>
+        <v>313</v>
       </c>
       <c r="D184" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>545</v>
+        <v>557</v>
       </c>
       <c r="B185" t="s">
         <v>59</v>
@@ -25414,13 +25428,13 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>548</v>
+        <v>560</v>
       </c>
       <c r="B186" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C186" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D186" t="s">
         <v>39</v>
@@ -25428,27 +25442,27 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>551</v>
+        <v>563</v>
       </c>
       <c r="B187" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C187" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D187" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>552</v>
+        <v>566</v>
       </c>
       <c r="B188" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C188" t="s">
-        <v>151</v>
+        <v>453</v>
       </c>
       <c r="D188" t="s">
         <v>39</v>
@@ -25456,27 +25470,27 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>553</v>
+        <v>567</v>
       </c>
       <c r="B189" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C189" t="s">
-        <v>313</v>
+        <v>184</v>
       </c>
       <c r="D189" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>557</v>
+        <v>570</v>
       </c>
       <c r="B190" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C190" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="D190" t="s">
         <v>39</v>
@@ -25484,13 +25498,13 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>560</v>
+        <v>573</v>
       </c>
       <c r="B191" t="s">
         <v>59</v>
       </c>
       <c r="C191" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D191" t="s">
         <v>39</v>
@@ -25498,27 +25512,27 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>563</v>
+        <v>576</v>
       </c>
       <c r="B192" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C192" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D192" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>566</v>
+        <v>577</v>
       </c>
       <c r="B193" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C193" t="s">
-        <v>453</v>
+        <v>291</v>
       </c>
       <c r="D193" t="s">
         <v>39</v>
@@ -25526,13 +25540,13 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>567</v>
+        <v>578</v>
       </c>
       <c r="B194" t="s">
         <v>59</v>
       </c>
       <c r="C194" t="s">
-        <v>184</v>
+        <v>65</v>
       </c>
       <c r="D194" t="s">
         <v>39</v>
@@ -25540,13 +25554,13 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>570</v>
+        <v>579</v>
       </c>
       <c r="B195" t="s">
         <v>69</v>
       </c>
       <c r="C195" t="s">
-        <v>128</v>
+        <v>353</v>
       </c>
       <c r="D195" t="s">
         <v>39</v>
@@ -25554,13 +25568,13 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>573</v>
+        <v>584</v>
       </c>
       <c r="B196" t="s">
         <v>59</v>
       </c>
       <c r="C196" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D196" t="s">
         <v>39</v>
@@ -25568,13 +25582,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>576</v>
+        <v>587</v>
       </c>
       <c r="B197" t="s">
         <v>59</v>
       </c>
       <c r="C197" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="D197" t="s">
         <v>39</v>
@@ -25582,13 +25596,13 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="B198" t="s">
         <v>59</v>
       </c>
       <c r="C198" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="D198" t="s">
         <v>39</v>
@@ -25596,13 +25610,13 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>578</v>
+        <v>591</v>
       </c>
       <c r="B199" t="s">
         <v>59</v>
       </c>
       <c r="C199" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="D199" t="s">
         <v>39</v>
@@ -25610,13 +25624,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>579</v>
+        <v>594</v>
       </c>
       <c r="B200" t="s">
         <v>69</v>
       </c>
       <c r="C200" t="s">
-        <v>353</v>
+        <v>162</v>
       </c>
       <c r="D200" t="s">
         <v>39</v>
@@ -25624,24 +25638,27 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>580</v>
+        <v>597</v>
       </c>
       <c r="B201" t="s">
-        <v>366</v>
+        <v>35</v>
+      </c>
+      <c r="C201" t="s">
+        <v>115</v>
       </c>
       <c r="D201" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>584</v>
+        <v>600</v>
       </c>
       <c r="B202" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C202" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D202" t="s">
         <v>39</v>
@@ -25649,13 +25666,13 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>587</v>
+        <v>603</v>
       </c>
       <c r="B203" t="s">
         <v>59</v>
       </c>
       <c r="C203" t="s">
-        <v>151</v>
+        <v>93</v>
       </c>
       <c r="D203" t="s">
         <v>39</v>
@@ -25663,13 +25680,13 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>588</v>
+        <v>606</v>
       </c>
       <c r="B204" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C204" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D204" t="s">
         <v>39</v>
@@ -25677,13 +25694,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>591</v>
+        <v>607</v>
       </c>
       <c r="B205" t="s">
         <v>59</v>
       </c>
       <c r="C205" t="s">
-        <v>93</v>
+        <v>250</v>
       </c>
       <c r="D205" t="s">
         <v>39</v>
@@ -25691,7 +25708,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>594</v>
+        <v>610</v>
       </c>
       <c r="B206" t="s">
         <v>69</v>
@@ -25705,10 +25722,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>597</v>
+        <v>611</v>
       </c>
       <c r="B207" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C207" t="s">
         <v>115</v>
@@ -25719,13 +25736,13 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>600</v>
+        <v>612</v>
       </c>
       <c r="B208" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C208" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="D208" t="s">
         <v>39</v>
@@ -25733,13 +25750,13 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>603</v>
+        <v>613</v>
       </c>
       <c r="B209" t="s">
         <v>59</v>
       </c>
       <c r="C209" t="s">
-        <v>93</v>
+        <v>317</v>
       </c>
       <c r="D209" t="s">
         <v>39</v>
@@ -25747,13 +25764,13 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="B210" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C210" t="s">
-        <v>315</v>
+        <v>186</v>
       </c>
       <c r="D210" t="s">
         <v>39</v>
@@ -25761,13 +25778,13 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>607</v>
+        <v>617</v>
       </c>
       <c r="B211" t="s">
         <v>59</v>
       </c>
       <c r="C211" t="s">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="D211" t="s">
         <v>39</v>
@@ -25775,13 +25792,13 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="B212" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C212" t="s">
-        <v>162</v>
+        <v>353</v>
       </c>
       <c r="D212" t="s">
         <v>39</v>
@@ -25789,13 +25806,13 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>611</v>
+        <v>621</v>
       </c>
       <c r="B213" t="s">
         <v>59</v>
       </c>
       <c r="C213" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="D213" t="s">
         <v>39</v>
@@ -25803,13 +25820,13 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="B214" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C214" t="s">
-        <v>190</v>
+        <v>128</v>
       </c>
       <c r="D214" t="s">
         <v>39</v>
@@ -25817,13 +25834,13 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>613</v>
+        <v>623</v>
       </c>
       <c r="B215" t="s">
         <v>59</v>
       </c>
       <c r="C215" t="s">
-        <v>317</v>
+        <v>151</v>
       </c>
       <c r="D215" t="s">
         <v>39</v>
@@ -25831,27 +25848,27 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>614</v>
+        <v>626</v>
       </c>
       <c r="B216" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C216" t="s">
-        <v>186</v>
+        <v>313</v>
       </c>
       <c r="D216" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>617</v>
+        <v>628</v>
       </c>
       <c r="B217" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C217" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="D217" t="s">
         <v>39</v>
@@ -25859,13 +25876,13 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="B218" t="s">
         <v>59</v>
       </c>
       <c r="C218" t="s">
-        <v>353</v>
+        <v>113</v>
       </c>
       <c r="D218" t="s">
         <v>39</v>
@@ -25873,13 +25890,13 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>621</v>
+        <v>632</v>
       </c>
       <c r="B219" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C219" t="s">
-        <v>204</v>
+        <v>353</v>
       </c>
       <c r="D219" t="s">
         <v>39</v>
@@ -25887,27 +25904,27 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>622</v>
+        <v>633</v>
       </c>
       <c r="B220" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C220" t="s">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="D220" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>623</v>
+        <v>635</v>
       </c>
       <c r="B221" t="s">
         <v>59</v>
       </c>
       <c r="C221" t="s">
-        <v>151</v>
+        <v>67</v>
       </c>
       <c r="D221" t="s">
         <v>39</v>
@@ -25915,38 +25932,41 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>626</v>
+        <v>636</v>
       </c>
       <c r="B222" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C222" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D222" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>627</v>
+        <v>639</v>
       </c>
       <c r="B223" t="s">
-        <v>78</v>
+        <v>91</v>
+      </c>
+      <c r="C223" t="s">
+        <v>151</v>
       </c>
       <c r="D223" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>628</v>
+        <v>641</v>
       </c>
       <c r="B224" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C224" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="D224" t="s">
         <v>39</v>
@@ -25954,13 +25974,13 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>629</v>
+        <v>642</v>
       </c>
       <c r="B225" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C225" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="D225" t="s">
         <v>39</v>
@@ -25968,41 +25988,41 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>632</v>
+        <v>645</v>
       </c>
       <c r="B226" t="s">
-        <v>69</v>
+        <v>366</v>
       </c>
       <c r="C226" t="s">
-        <v>353</v>
+        <v>647</v>
       </c>
       <c r="D226" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>633</v>
+        <v>648</v>
       </c>
       <c r="B227" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C227" t="s">
-        <v>52</v>
+        <v>177</v>
       </c>
       <c r="D227" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>635</v>
+        <v>649</v>
       </c>
       <c r="B228" t="s">
         <v>59</v>
       </c>
       <c r="C228" t="s">
-        <v>67</v>
+        <v>200</v>
       </c>
       <c r="D228" t="s">
         <v>39</v>
@@ -26010,27 +26030,27 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>636</v>
+        <v>650</v>
       </c>
       <c r="B229" t="s">
-        <v>35</v>
+        <v>366</v>
       </c>
       <c r="C229" t="s">
-        <v>302</v>
+        <v>653</v>
       </c>
       <c r="D229" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>639</v>
+        <v>655</v>
       </c>
       <c r="B230" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C230" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="D230" t="s">
         <v>39</v>
@@ -26038,13 +26058,13 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>641</v>
+        <v>658</v>
       </c>
       <c r="B231" t="s">
         <v>59</v>
       </c>
       <c r="C231" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="D231" t="s">
         <v>39</v>
@@ -26052,13 +26072,13 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>642</v>
+        <v>659</v>
       </c>
       <c r="B232" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C232" t="s">
-        <v>128</v>
+        <v>341</v>
       </c>
       <c r="D232" t="s">
         <v>39</v>
@@ -26066,69 +26086,69 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>645</v>
+        <v>662</v>
       </c>
       <c r="B233" t="s">
-        <v>366</v>
+        <v>59</v>
       </c>
       <c r="C233" t="s">
-        <v>647</v>
+        <v>421</v>
       </c>
       <c r="D233" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>648</v>
+        <v>665</v>
       </c>
       <c r="B234" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C234" t="s">
-        <v>177</v>
+        <v>37</v>
       </c>
       <c r="D234" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>649</v>
+        <v>668</v>
       </c>
       <c r="B235" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C235" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="D235" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>650</v>
+        <v>672</v>
       </c>
       <c r="B236" t="s">
-        <v>366</v>
+        <v>69</v>
       </c>
       <c r="C236" t="s">
-        <v>653</v>
+        <v>291</v>
       </c>
       <c r="D236" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>655</v>
+        <v>675</v>
       </c>
       <c r="B237" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C237" t="s">
-        <v>99</v>
+        <v>278</v>
       </c>
       <c r="D237" t="s">
         <v>39</v>
@@ -26136,27 +26156,27 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>658</v>
+        <v>678</v>
       </c>
       <c r="B238" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C238" t="s">
-        <v>190</v>
+        <v>52</v>
       </c>
       <c r="D238" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>659</v>
+        <v>680</v>
       </c>
       <c r="B239" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C239" t="s">
-        <v>341</v>
+        <v>421</v>
       </c>
       <c r="D239" t="s">
         <v>39</v>
@@ -26164,13 +26184,13 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>662</v>
+        <v>681</v>
       </c>
       <c r="B240" t="s">
         <v>59</v>
       </c>
       <c r="C240" t="s">
-        <v>421</v>
+        <v>204</v>
       </c>
       <c r="D240" t="s">
         <v>39</v>
@@ -26178,41 +26198,41 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>665</v>
+        <v>684</v>
       </c>
       <c r="B241" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C241" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="D241" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>668</v>
+        <v>685</v>
       </c>
       <c r="B242" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C242" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
       <c r="D242" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>672</v>
+        <v>688</v>
       </c>
       <c r="B243" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C243" t="s">
-        <v>291</v>
+        <v>200</v>
       </c>
       <c r="D243" t="s">
         <v>39</v>
@@ -26220,13 +26240,13 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>675</v>
+        <v>689</v>
       </c>
       <c r="B244" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="C244" t="s">
-        <v>278</v>
+        <v>177</v>
       </c>
       <c r="D244" t="s">
         <v>39</v>
@@ -26234,55 +26254,55 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>678</v>
+        <v>692</v>
       </c>
       <c r="B245" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C245" t="s">
-        <v>52</v>
+        <v>278</v>
       </c>
       <c r="D245" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>680</v>
+        <v>695</v>
       </c>
       <c r="B246" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C246" t="s">
-        <v>421</v>
+        <v>37</v>
       </c>
       <c r="D246" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>681</v>
+        <v>698</v>
       </c>
       <c r="B247" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C247" t="s">
-        <v>204</v>
+        <v>653</v>
       </c>
       <c r="D247" t="s">
-        <v>39</v>
+        <v>699</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>684</v>
+        <v>701</v>
       </c>
       <c r="B248" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C248" t="s">
-        <v>71</v>
+        <v>186</v>
       </c>
       <c r="D248" t="s">
         <v>39</v>
@@ -26290,13 +26310,13 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>685</v>
+        <v>702</v>
       </c>
       <c r="B249" t="s">
         <v>59</v>
       </c>
       <c r="C249" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="D249" t="s">
         <v>39</v>
@@ -26304,13 +26324,13 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>688</v>
+        <v>703</v>
       </c>
       <c r="B250" t="s">
         <v>59</v>
       </c>
       <c r="C250" t="s">
-        <v>200</v>
+        <v>61</v>
       </c>
       <c r="D250" t="s">
         <v>39</v>
@@ -26318,13 +26338,13 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>689</v>
+        <v>704</v>
       </c>
       <c r="B251" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C251" t="s">
-        <v>177</v>
+        <v>105</v>
       </c>
       <c r="D251" t="s">
         <v>39</v>
@@ -26332,13 +26352,13 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>692</v>
+        <v>707</v>
       </c>
       <c r="B252" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C252" t="s">
-        <v>278</v>
+        <v>44</v>
       </c>
       <c r="D252" t="s">
         <v>39</v>
@@ -26346,41 +26366,41 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>695</v>
+        <v>708</v>
       </c>
       <c r="B253" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C253" t="s">
-        <v>37</v>
+        <v>151</v>
       </c>
       <c r="D253" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>698</v>
+        <v>709</v>
       </c>
       <c r="B254" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C254" t="s">
-        <v>653</v>
+        <v>505</v>
       </c>
       <c r="D254" t="s">
-        <v>699</v>
+        <v>39</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>701</v>
+        <v>712</v>
       </c>
       <c r="B255" t="s">
         <v>59</v>
       </c>
       <c r="C255" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="D255" t="s">
         <v>39</v>
@@ -26388,13 +26408,13 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="B256" t="s">
         <v>59</v>
       </c>
       <c r="C256" t="s">
-        <v>250</v>
+        <v>65</v>
       </c>
       <c r="D256" t="s">
         <v>39</v>
@@ -26402,27 +26422,27 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>703</v>
+        <v>717</v>
       </c>
       <c r="B257" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C257" t="s">
-        <v>61</v>
+        <v>250</v>
       </c>
       <c r="D257" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>704</v>
+        <v>720</v>
       </c>
       <c r="B258" t="s">
         <v>59</v>
       </c>
       <c r="C258" t="s">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="D258" t="s">
         <v>39</v>
@@ -26430,13 +26450,13 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>707</v>
+        <v>721</v>
       </c>
       <c r="B259" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="C259" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="D259" t="s">
         <v>39</v>
@@ -26444,13 +26464,13 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>708</v>
+        <v>724</v>
       </c>
       <c r="B260" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C260" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="D260" t="s">
         <v>39</v>
@@ -26458,13 +26478,13 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>709</v>
+        <v>725</v>
       </c>
       <c r="B261" t="s">
         <v>59</v>
       </c>
       <c r="C261" t="s">
-        <v>505</v>
+        <v>128</v>
       </c>
       <c r="D261" t="s">
         <v>39</v>
@@ -26472,13 +26492,13 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>712</v>
+        <v>728</v>
       </c>
       <c r="B262" t="s">
         <v>59</v>
       </c>
       <c r="C262" t="s">
-        <v>151</v>
+        <v>375</v>
       </c>
       <c r="D262" t="s">
         <v>39</v>
@@ -26486,13 +26506,13 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>715</v>
+        <v>731</v>
       </c>
       <c r="B263" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C263" t="s">
-        <v>65</v>
+        <v>315</v>
       </c>
       <c r="D263" t="s">
         <v>39</v>
@@ -26500,27 +26520,27 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>717</v>
+        <v>732</v>
       </c>
       <c r="B264" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="C264" t="s">
-        <v>250</v>
+        <v>109</v>
       </c>
       <c r="D264" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>720</v>
+        <v>733</v>
       </c>
       <c r="B265" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C265" t="s">
-        <v>204</v>
+        <v>109</v>
       </c>
       <c r="D265" t="s">
         <v>39</v>
@@ -26528,27 +26548,27 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>721</v>
+        <v>736</v>
       </c>
       <c r="B266" t="s">
-        <v>59</v>
+        <v>366</v>
       </c>
       <c r="C266" t="s">
-        <v>175</v>
+        <v>45</v>
       </c>
       <c r="D266" t="s">
-        <v>39</v>
+        <v>741</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>724</v>
+        <v>744</v>
       </c>
       <c r="B267" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C267" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="D267" t="s">
         <v>39</v>
@@ -26556,13 +26576,13 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>725</v>
+        <v>745</v>
       </c>
       <c r="B268" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="C268" t="s">
-        <v>128</v>
+        <v>415</v>
       </c>
       <c r="D268" t="s">
         <v>39</v>
@@ -26570,13 +26590,13 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>728</v>
+        <v>747</v>
       </c>
       <c r="B269" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C269" t="s">
-        <v>375</v>
+        <v>484</v>
       </c>
       <c r="D269" t="s">
         <v>39</v>
@@ -26584,13 +26604,13 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>731</v>
+        <v>748</v>
       </c>
       <c r="B270" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C270" t="s">
-        <v>315</v>
+        <v>155</v>
       </c>
       <c r="D270" t="s">
         <v>39</v>
@@ -26598,13 +26618,13 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>732</v>
+        <v>749</v>
       </c>
       <c r="B271" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C271" t="s">
-        <v>109</v>
+        <v>750</v>
       </c>
       <c r="D271" t="s">
         <v>39</v>
@@ -26612,13 +26632,13 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>733</v>
+        <v>751</v>
       </c>
       <c r="B272" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C272" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D272" t="s">
         <v>39</v>
@@ -26626,27 +26646,27 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>736</v>
+        <v>752</v>
       </c>
       <c r="B273" t="s">
-        <v>366</v>
+        <v>59</v>
       </c>
       <c r="C273" t="s">
-        <v>45</v>
+        <v>291</v>
       </c>
       <c r="D273" t="s">
-        <v>741</v>
+        <v>39</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>744</v>
+        <v>755</v>
       </c>
       <c r="B274" t="s">
         <v>59</v>
       </c>
       <c r="C274" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="D274" t="s">
         <v>39</v>
@@ -26654,27 +26674,27 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>745</v>
+        <v>756</v>
       </c>
       <c r="B275" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="C275" t="s">
-        <v>415</v>
+        <v>37</v>
       </c>
       <c r="D275" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>747</v>
+        <v>760</v>
       </c>
       <c r="B276" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C276" t="s">
-        <v>484</v>
+        <v>126</v>
       </c>
       <c r="D276" t="s">
         <v>39</v>
@@ -26682,13 +26702,13 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>748</v>
+        <v>763</v>
       </c>
       <c r="B277" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C277" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="D277" t="s">
         <v>39</v>
@@ -26696,13 +26716,13 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>749</v>
+        <v>766</v>
       </c>
       <c r="B278" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C278" t="s">
-        <v>750</v>
+        <v>115</v>
       </c>
       <c r="D278" t="s">
         <v>39</v>
@@ -26710,13 +26730,13 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>751</v>
+        <v>769</v>
       </c>
       <c r="B279" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C279" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="D279" t="s">
         <v>39</v>
@@ -26724,13 +26744,13 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>752</v>
+        <v>770</v>
       </c>
       <c r="B280" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C280" t="s">
-        <v>291</v>
+        <v>132</v>
       </c>
       <c r="D280" t="s">
         <v>39</v>
@@ -26738,13 +26758,13 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>755</v>
+        <v>771</v>
       </c>
       <c r="B281" t="s">
         <v>59</v>
       </c>
       <c r="C281" t="s">
-        <v>71</v>
+        <v>348</v>
       </c>
       <c r="D281" t="s">
         <v>39</v>
@@ -26752,27 +26772,27 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>756</v>
+        <v>772</v>
       </c>
       <c r="B282" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C282" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="D282" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="B283" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C283" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="D283" t="s">
         <v>39</v>
@@ -26780,113 +26800,15 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>763</v>
+        <v>776</v>
       </c>
       <c r="B284" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C284" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D284" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A285" t="s">
-        <v>766</v>
-      </c>
-      <c r="B285" t="s">
-        <v>59</v>
-      </c>
-      <c r="C285" t="s">
-        <v>115</v>
-      </c>
-      <c r="D285" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A286" t="s">
-        <v>769</v>
-      </c>
-      <c r="B286" t="s">
-        <v>69</v>
-      </c>
-      <c r="C286" t="s">
-        <v>162</v>
-      </c>
-      <c r="D286" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A287" t="s">
-        <v>770</v>
-      </c>
-      <c r="B287" t="s">
-        <v>69</v>
-      </c>
-      <c r="C287" t="s">
-        <v>132</v>
-      </c>
-      <c r="D287" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A288" t="s">
-        <v>771</v>
-      </c>
-      <c r="B288" t="s">
-        <v>59</v>
-      </c>
-      <c r="C288" t="s">
-        <v>348</v>
-      </c>
-      <c r="D288" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A289" t="s">
-        <v>772</v>
-      </c>
-      <c r="B289" t="s">
-        <v>59</v>
-      </c>
-      <c r="C289" t="s">
-        <v>132</v>
-      </c>
-      <c r="D289" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A290" t="s">
-        <v>773</v>
-      </c>
-      <c r="B290" t="s">
-        <v>59</v>
-      </c>
-      <c r="C290" t="s">
-        <v>99</v>
-      </c>
-      <c r="D290" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A291" t="s">
-        <v>776</v>
-      </c>
-      <c r="B291" t="s">
-        <v>59</v>
-      </c>
-      <c r="C291" t="s">
-        <v>115</v>
-      </c>
-      <c r="D291" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
still stuck at moving col
</commit_message>
<xml_diff>
--- a/Vehicle information_20240728_213917.xlsx
+++ b/Vehicle information_20240728_213917.xlsx
@@ -19,9 +19,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
       <sz val="10"/>
     </font>
     <font>
@@ -101,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -109,10 +114,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -515,8 +523,8 @@
   <dimension ref="A1:AC291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B82" sqref="B81:B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -31533,22 +31541,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>VIN</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Vehicle series name</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Delivery date</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Target country for vehicle sales</t>
         </is>

</xml_diff>

<commit_message>
BUG, worksheet must be saved first to make another move
</commit_message>
<xml_diff>
--- a/Vehicle information_20240728_213917.xlsx
+++ b/Vehicle information_20240728_213917.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle information" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,19 +19,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <b val="1"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <b val="1"/>
       <sz val="10"/>
     </font>
     <font>
@@ -58,7 +48,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -82,21 +72,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -106,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -114,13 +89,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -522,8 +491,8 @@
   </sheetPr>
   <dimension ref="A1:AC291"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B82" sqref="B81:B82"/>
     </sheetView>
   </sheetViews>
@@ -31541,22 +31510,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>VIN</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Vehicle series name</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Delivery date</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Target country for vehicle sales</t>
         </is>

</xml_diff>